<commit_message>
Datos camino video 30
</commit_message>
<xml_diff>
--- a/datos_mov_browniano.xlsx
+++ b/datos_mov_browniano.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javier/Documents/University/5th_semester/Experimental physics/Unidad4_MovBrowniano/Videos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javier/Documents/University/5th_semester/Experimental_physics/Unidad4_MovBrowniano/Videos/manejo_datos_U4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39ACCF7-91DF-7D48-A46E-2ACCA25A1F54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE0F8E4-D644-A044-91B4-3C119DDD1880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="440" windowWidth="24820" windowHeight="15020" xr2:uid="{A3EB2B8F-6FDE-E74E-A681-BB9E867116F0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>t30</t>
   </si>
@@ -214,6 +214,15 @@
   </si>
   <si>
     <t>r10</t>
+  </si>
+  <si>
+    <t>t_path_30</t>
+  </si>
+  <si>
+    <t>x_path_30</t>
+  </si>
+  <si>
+    <t>y_path_30</t>
   </si>
 </sst>
 </file>
@@ -566,15 +575,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1721A824-AADC-CF47-B5FD-042022608B71}">
-  <dimension ref="A1:BH201"/>
+  <dimension ref="A1:BK201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AN7" sqref="AN7"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BK6" sqref="BK6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,8 +764,17 @@
       <c r="BH1" t="s">
         <v>58</v>
       </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -937,8 +955,17 @@
       <c r="BH2" s="1">
         <v>4.3733335059999998E-5</v>
       </c>
+      <c r="BI2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="1">
+        <v>-2.1261514709999999E-5</v>
+      </c>
+      <c r="BK2" s="1">
+        <v>6.3163554119999998E-5</v>
+      </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.2</v>
       </c>
@@ -1119,8 +1146,17 @@
       <c r="BH3" s="1">
         <v>1.1938673339999999E-3</v>
       </c>
+      <c r="BI3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="BJ3" s="1">
+        <v>-1.3424868779999999E-3</v>
+      </c>
+      <c r="BK3" s="1">
+        <v>1.099444748E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.4</v>
       </c>
@@ -1301,8 +1337,17 @@
       <c r="BH4" s="1">
         <v>1.522630187E-3</v>
       </c>
+      <c r="BI4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="BJ4" s="1">
+        <v>-5.8799391659999998E-4</v>
+      </c>
+      <c r="BK4" s="1">
+        <v>1.028041416E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.6</v>
       </c>
@@ -1483,8 +1528,17 @@
       <c r="BH5" s="1">
         <v>3.2792025390000002E-3</v>
       </c>
+      <c r="BI5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="BJ5" s="1">
+        <v>-4.2602694009999999E-4</v>
+      </c>
+      <c r="BK5" s="1">
+        <v>-9.078318744E-4</v>
+      </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.8</v>
       </c>
@@ -1665,8 +1719,17 @@
       <c r="BH6" s="1">
         <v>3.185788141E-3</v>
       </c>
+      <c r="BI6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="BJ6" s="1">
+        <v>9.2503533619999999E-5</v>
+      </c>
+      <c r="BK6" s="1">
+        <v>-2.049914096E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1847,8 +1910,17 @@
       <c r="BH7" s="1">
         <v>3.1828055369999999E-3</v>
       </c>
+      <c r="BI7" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ7" s="1">
+        <v>-2.3573525729999999E-3</v>
+      </c>
+      <c r="BK7" s="1">
+        <v>-2.0564290420000001E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1.2</v>
       </c>
@@ -2029,8 +2101,17 @@
       <c r="BH8" s="1">
         <v>3.8052815369999998E-3</v>
       </c>
+      <c r="BI8" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="BJ8" s="1">
+        <v>-1.4445341039999999E-3</v>
+      </c>
+      <c r="BK8" s="1">
+        <v>-2.5087628869999998E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -2211,8 +2292,17 @@
       <c r="BH9" s="1">
         <v>4.5846016450000002E-3</v>
       </c>
+      <c r="BI9" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="BJ9" s="1">
+        <v>-1.1009692459999999E-3</v>
+      </c>
+      <c r="BK9" s="1">
+        <v>-1.2586910599999999E-3</v>
+      </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1.6</v>
       </c>
@@ -2393,8 +2483,17 @@
       <c r="BH10" s="1">
         <v>4.9198320980000003E-3</v>
       </c>
+      <c r="BI10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="BJ10" s="1">
+        <v>-7.6718391199999999E-4</v>
+      </c>
+      <c r="BK10" s="1">
+        <v>-9.5689521420000003E-5</v>
+      </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1.8</v>
       </c>
@@ -2575,8 +2674,17 @@
       <c r="BH11" s="1">
         <v>6.5907578830000004E-3</v>
       </c>
+      <c r="BI11" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="BJ11" s="1">
+        <v>5.1067052950000001E-4</v>
+      </c>
+      <c r="BK11" s="1">
+        <v>-6.4045012410000001E-4</v>
+      </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -2757,8 +2865,17 @@
       <c r="BH12" s="1">
         <v>5.5053856630000002E-3</v>
       </c>
+      <c r="BI12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ12" s="1">
+        <v>1.468525224E-3</v>
+      </c>
+      <c r="BK12" s="1">
+        <v>-1.60032292E-3</v>
+      </c>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -2939,8 +3056,17 @@
       <c r="BH13" s="1">
         <v>5.6528487759999997E-3</v>
       </c>
+      <c r="BI13" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BJ13" s="1">
+        <v>4.3813786349999997E-4</v>
+      </c>
+      <c r="BK13" s="1">
+        <v>-1.419718046E-3</v>
+      </c>
     </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2.4</v>
       </c>
@@ -3121,8 +3247,17 @@
       <c r="BH14" s="1">
         <v>4.9167536589999998E-3</v>
       </c>
+      <c r="BI14" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="BJ14" s="1">
+        <v>3.254210076E-4</v>
+      </c>
+      <c r="BK14" s="1">
+        <v>-1.6550153380000001E-3</v>
+      </c>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2.6</v>
       </c>
@@ -3303,8 +3438,17 @@
       <c r="BH15" s="1">
         <v>2.5216207440000001E-3</v>
       </c>
+      <c r="BI15" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="BJ15" s="1">
+        <v>-4.2186240870000001E-4</v>
+      </c>
+      <c r="BK15" s="1">
+        <v>-1.6462295419999999E-3</v>
+      </c>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2.8</v>
       </c>
@@ -3485,8 +3629,17 @@
       <c r="BH16" s="1">
         <v>3.1786112000000001E-3</v>
       </c>
+      <c r="BI16" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="BJ16" s="1">
+        <v>6.181532061E-4</v>
+      </c>
+      <c r="BK16" s="1">
+        <v>-1.727049389E-3</v>
+      </c>
     </row>
-    <row r="17" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -3667,8 +3820,17 @@
       <c r="BH17" s="1">
         <v>3.9932350060000003E-3</v>
       </c>
+      <c r="BI17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BJ17" s="1">
+        <v>4.967337284E-4</v>
+      </c>
+      <c r="BK17" s="1">
+        <v>-3.6581651940000002E-3</v>
+      </c>
     </row>
-    <row r="18" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>3.2</v>
       </c>
@@ -3849,8 +4011,17 @@
       <c r="BH18" s="1">
         <v>6.1357556900000004E-3</v>
       </c>
+      <c r="BI18" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="BJ18" s="1">
+        <v>1.9227217409999999E-3</v>
+      </c>
+      <c r="BK18" s="1">
+        <v>-4.8509137439999997E-3</v>
+      </c>
     </row>
-    <row r="19" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>3.4</v>
       </c>
@@ -4031,8 +4202,17 @@
       <c r="BH19" s="1">
         <v>7.2682092709999997E-3</v>
       </c>
+      <c r="BI19" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="BJ19" s="1">
+        <v>2.8326870249999999E-3</v>
+      </c>
+      <c r="BK19" s="1">
+        <v>-3.8184348869999998E-3</v>
+      </c>
     </row>
-    <row r="20" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>3.6</v>
       </c>
@@ -4213,8 +4393,17 @@
       <c r="BH20" s="1">
         <v>7.1491948580000002E-3</v>
       </c>
+      <c r="BI20" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="BJ20" s="1">
+        <v>3.4635335869999998E-3</v>
+      </c>
+      <c r="BK20" s="1">
+        <v>-4.7411951179999997E-3</v>
+      </c>
     </row>
-    <row r="21" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>3.8</v>
       </c>
@@ -4395,8 +4584,17 @@
       <c r="BH21" s="1">
         <v>6.9435478190000002E-3</v>
       </c>
+      <c r="BI21" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="BJ21" s="1">
+        <v>3.7975841549999999E-3</v>
+      </c>
+      <c r="BK21" s="1">
+        <v>-5.3492502639999997E-3</v>
+      </c>
     </row>
-    <row r="22" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -4577,8 +4775,17 @@
       <c r="BH22" s="1">
         <v>8.6091935190000003E-3</v>
       </c>
+      <c r="BI22" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ22" s="1">
+        <v>6.2586458849999997E-3</v>
+      </c>
+      <c r="BK22" s="1">
+        <v>-3.9351985609999999E-3</v>
+      </c>
     </row>
-    <row r="23" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>4.2</v>
       </c>
@@ -4759,8 +4966,17 @@
       <c r="BH23" s="1">
         <v>9.5219370840000008E-3</v>
       </c>
+      <c r="BI23" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="BJ23" s="1">
+        <v>6.661255003E-3</v>
+      </c>
+      <c r="BK23" s="1">
+        <v>-4.1737141359999997E-3</v>
+      </c>
     </row>
-    <row r="24" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>4.4000000000000004</v>
       </c>
@@ -4941,8 +5157,17 @@
       <c r="BH24" s="1">
         <v>9.2286790650000002E-3</v>
       </c>
+      <c r="BI24" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="BJ24" s="1">
+        <v>6.539347442E-3</v>
+      </c>
+      <c r="BK24" s="1">
+        <v>-4.4479082709999998E-3</v>
+      </c>
     </row>
-    <row r="25" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>4.5999999999999996</v>
       </c>
@@ -5123,8 +5348,17 @@
       <c r="BH25" s="1">
         <v>9.450380546E-3</v>
       </c>
+      <c r="BI25" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="BJ25" s="1">
+        <v>6.1947962250000002E-3</v>
+      </c>
+      <c r="BK25" s="1">
+        <v>-2.9552804540000002E-3</v>
+      </c>
     </row>
-    <row r="26" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>4.8</v>
       </c>
@@ -5305,8 +5539,17 @@
       <c r="BH26" s="1">
         <v>1.0237705640000001E-2</v>
       </c>
+      <c r="BI26" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="BJ26" s="1">
+        <v>5.9733923030000002E-3</v>
+      </c>
+      <c r="BK26" s="1">
+        <v>-3.0317443760000001E-3</v>
+      </c>
     </row>
-    <row r="27" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>5</v>
       </c>
@@ -5487,8 +5730,17 @@
       <c r="BH27" s="1">
         <v>1.044600541E-2</v>
       </c>
+      <c r="BI27" s="1">
+        <v>5</v>
+      </c>
+      <c r="BJ27" s="1">
+        <v>5.9168114469999996E-3</v>
+      </c>
+      <c r="BK27" s="1">
+        <v>-2.6902515600000002E-3</v>
+      </c>
     </row>
-    <row r="28" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>5.2</v>
       </c>
@@ -5669,8 +5921,17 @@
       <c r="BH28" s="1">
         <v>9.8870815800000001E-3</v>
       </c>
+      <c r="BI28" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="BJ28" s="1">
+        <v>4.3706385799999999E-3</v>
+      </c>
+      <c r="BK28" s="1">
+        <v>-2.3889508879999998E-3</v>
+      </c>
     </row>
-    <row r="29" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>5.4</v>
       </c>
@@ -5851,8 +6112,17 @@
       <c r="BH29" s="1">
         <v>1.016710807E-2</v>
       </c>
+      <c r="BI29" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="BJ29" s="1">
+        <v>4.0327672920000002E-3</v>
+      </c>
+      <c r="BK29" s="1">
+        <v>-2.6317768860000001E-3</v>
+      </c>
     </row>
-    <row r="30" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>5.6</v>
       </c>
@@ -6033,8 +6303,17 @@
       <c r="BH30" s="1">
         <v>8.6695026829999994E-3</v>
       </c>
+      <c r="BI30" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="BJ30" s="1">
+        <v>3.6634435099999999E-3</v>
+      </c>
+      <c r="BK30" s="1">
+        <v>-1.964510774E-3</v>
+      </c>
     </row>
-    <row r="31" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>5.8</v>
       </c>
@@ -6215,8 +6494,17 @@
       <c r="BH31" s="1">
         <v>1.019297158E-2</v>
       </c>
+      <c r="BI31" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="BJ31" s="1">
+        <v>4.1432322269999997E-3</v>
+      </c>
+      <c r="BK31" s="1">
+        <v>-1.250071748E-3</v>
+      </c>
     </row>
-    <row r="32" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>6</v>
       </c>
@@ -6397,8 +6685,17 @@
       <c r="BH32" s="1">
         <v>9.1657576060000003E-3</v>
       </c>
+      <c r="BI32" s="1">
+        <v>6</v>
+      </c>
+      <c r="BJ32" s="1">
+        <v>2.8293478849999998E-3</v>
+      </c>
+      <c r="BK32" s="1">
+        <v>2.956647507E-4</v>
+      </c>
     </row>
-    <row r="33" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>6.2</v>
       </c>
@@ -6579,8 +6876,17 @@
       <c r="BH33" s="1">
         <v>7.5629083019999998E-3</v>
       </c>
+      <c r="BI33" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="BJ33" s="1">
+        <v>2.777833104E-3</v>
+      </c>
+      <c r="BK33" s="1">
+        <v>-1.7180451949999999E-4</v>
+      </c>
     </row>
-    <row r="34" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>6.4</v>
       </c>
@@ -6761,8 +7067,17 @@
       <c r="BH34" s="1">
         <v>6.9830462629999999E-3</v>
       </c>
+      <c r="BI34" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="BJ34" s="1">
+        <v>2.0327466339999998E-3</v>
+      </c>
+      <c r="BK34" s="1">
+        <v>3.4925777039999999E-4</v>
+      </c>
     </row>
-    <row r="35" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>6.6</v>
       </c>
@@ -6943,8 +7258,17 @@
       <c r="BH35" s="1">
         <v>6.7503127580000001E-3</v>
       </c>
+      <c r="BI35" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="BJ35" s="1">
+        <v>2.3224775750000002E-3</v>
+      </c>
+      <c r="BK35" s="1">
+        <v>1.880819797E-3</v>
+      </c>
     </row>
-    <row r="36" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>6.8</v>
       </c>
@@ -7125,8 +7449,17 @@
       <c r="BH36" s="1">
         <v>6.0128891590000002E-3</v>
       </c>
+      <c r="BI36" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="BJ36" s="1">
+        <v>2.5972575960000002E-3</v>
+      </c>
+      <c r="BK36" s="1">
+        <v>2.1127651499999998E-3</v>
+      </c>
     </row>
-    <row r="37" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>7</v>
       </c>
@@ -7307,8 +7640,17 @@
       <c r="BH37" s="1">
         <v>3.538632302E-3</v>
       </c>
+      <c r="BI37" s="1">
+        <v>7</v>
+      </c>
+      <c r="BJ37" s="1">
+        <v>1.9751291459999998E-3</v>
+      </c>
+      <c r="BK37" s="1">
+        <v>2.3559650779999999E-3</v>
+      </c>
     </row>
-    <row r="38" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>7.2</v>
       </c>
@@ -7489,8 +7831,17 @@
       <c r="BH38" s="1">
         <v>2.9275176410000002E-3</v>
       </c>
+      <c r="BI38" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="BJ38" s="1">
+        <v>2.3679130980000002E-3</v>
+      </c>
+      <c r="BK38" s="1">
+        <v>2.7087514170000002E-3</v>
+      </c>
     </row>
-    <row r="39" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>7.4</v>
       </c>
@@ -7671,8 +8022,17 @@
       <c r="BH39" s="1">
         <v>4.1786130859999999E-3</v>
       </c>
+      <c r="BI39" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="BJ39" s="1">
+        <v>1.923435923E-3</v>
+      </c>
+      <c r="BK39" s="1">
+        <v>2.6815499630000001E-3</v>
+      </c>
     </row>
-    <row r="40" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>7.6</v>
       </c>
@@ -7853,8 +8213,17 @@
       <c r="BH40" s="1">
         <v>4.1705946690000001E-3</v>
       </c>
+      <c r="BI40" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="BJ40" s="1">
+        <v>1.5164873299999999E-3</v>
+      </c>
+      <c r="BK40" s="1">
+        <v>2.6281263170000002E-3</v>
+      </c>
     </row>
-    <row r="41" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>7.8</v>
       </c>
@@ -8035,8 +8404,17 @@
       <c r="BH41" s="1">
         <v>4.9686821139999999E-3</v>
       </c>
+      <c r="BI41" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="BJ41" s="1">
+        <v>4.9998540069999997E-4</v>
+      </c>
+      <c r="BK41" s="1">
+        <v>2.4962841080000001E-3</v>
+      </c>
     </row>
-    <row r="42" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>8</v>
       </c>
@@ -8217,8 +8595,17 @@
       <c r="BH42" s="1">
         <v>5.208509026E-3</v>
       </c>
+      <c r="BI42" s="1">
+        <v>8</v>
+      </c>
+      <c r="BJ42" s="1">
+        <v>2.7109907609999999E-3</v>
+      </c>
+      <c r="BK42" s="1">
+        <v>2.2490018099999998E-3</v>
+      </c>
     </row>
-    <row r="43" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>8.1999999999999993</v>
       </c>
@@ -8399,8 +8786,17 @@
       <c r="BH43" s="1">
         <v>4.23427154E-3</v>
       </c>
+      <c r="BI43" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="BJ43" s="1">
+        <v>3.6344898519999999E-3</v>
+      </c>
+      <c r="BK43" s="1">
+        <v>2.5047663840000001E-3</v>
+      </c>
     </row>
-    <row r="44" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>8.4</v>
       </c>
@@ -8581,8 +8977,17 @@
       <c r="BH44" s="1">
         <v>2.9507213419999998E-3</v>
       </c>
+      <c r="BI44" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="BJ44" s="1">
+        <v>6.1974179650000003E-3</v>
+      </c>
+      <c r="BK44" s="1">
+        <v>2.4788261439999998E-3</v>
+      </c>
     </row>
-    <row r="45" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>8.6</v>
       </c>
@@ -8763,8 +9168,17 @@
       <c r="BH45" s="1">
         <v>2.8269270500000001E-3</v>
       </c>
+      <c r="BI45" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="BJ45" s="1">
+        <v>7.7380294949999998E-3</v>
+      </c>
+      <c r="BK45" s="1">
+        <v>2.3563691150000001E-3</v>
+      </c>
     </row>
-    <row r="46" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>8.8000000000000007</v>
       </c>
@@ -8945,8 +9359,17 @@
       <c r="BH46" s="1">
         <v>3.663666936E-3</v>
       </c>
+      <c r="BI46" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="BJ46" s="1">
+        <v>8.1359417700000002E-3</v>
+      </c>
+      <c r="BK46" s="1">
+        <v>2.0144902079999999E-3</v>
+      </c>
     </row>
-    <row r="47" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>9</v>
       </c>
@@ -9127,8 +9550,17 @@
       <c r="BH47" s="1">
         <v>3.9185498869999998E-3</v>
       </c>
+      <c r="BI47" s="1">
+        <v>9</v>
+      </c>
+      <c r="BJ47" s="1">
+        <v>8.6594049240000005E-3</v>
+      </c>
+      <c r="BK47" s="1">
+        <v>1.4242673930000001E-3</v>
+      </c>
     </row>
-    <row r="48" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>9.1999999999999993</v>
       </c>
@@ -9309,8 +9741,17 @@
       <c r="BH48" s="1">
         <v>3.9324444280000002E-3</v>
       </c>
+      <c r="BI48" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="BJ48" s="1">
+        <v>9.2760752840000005E-3</v>
+      </c>
+      <c r="BK48" s="1">
+        <v>1.5862481280000001E-3</v>
+      </c>
     </row>
-    <row r="49" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>9.4</v>
       </c>
@@ -9491,8 +9932,17 @@
       <c r="BH49" s="1">
         <v>2.476161475E-3</v>
       </c>
+      <c r="BI49" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="BJ49" s="1">
+        <v>8.3639747619999993E-3</v>
+      </c>
+      <c r="BK49" s="1">
+        <v>1.3926941180000001E-3</v>
+      </c>
     </row>
-    <row r="50" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>9.6</v>
       </c>
@@ -9673,8 +10123,17 @@
       <c r="BH50" s="1">
         <v>1.904807306E-3</v>
       </c>
+      <c r="BI50" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="BJ50" s="1">
+        <v>7.2285625980000002E-3</v>
+      </c>
+      <c r="BK50" s="1">
+        <v>1.6511057149999999E-3</v>
+      </c>
     </row>
-    <row r="51" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>9.8000000000000007</v>
       </c>
@@ -9855,8 +10314,17 @@
       <c r="BH51" s="1">
         <v>2.574743539E-3</v>
       </c>
+      <c r="BI51" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="BJ51" s="1">
+        <v>7.5144740009999997E-3</v>
+      </c>
+      <c r="BK51" s="1">
+        <v>1.4315496299999999E-3</v>
+      </c>
     </row>
-    <row r="52" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>10</v>
       </c>
@@ -10037,8 +10505,17 @@
       <c r="BH52" s="1">
         <v>3.9923953949999999E-3</v>
       </c>
+      <c r="BI52" s="1">
+        <v>10</v>
+      </c>
+      <c r="BJ52" s="1">
+        <v>7.7448430100000003E-3</v>
+      </c>
+      <c r="BK52" s="1">
+        <v>1.5957441560000001E-3</v>
+      </c>
     </row>
-    <row r="53" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>10.199999999999999</v>
       </c>
@@ -10219,8 +10696,17 @@
       <c r="BH53" s="1">
         <v>4.6671009440000001E-3</v>
       </c>
+      <c r="BI53" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="BJ53" s="1">
+        <v>6.9957767060000002E-3</v>
+      </c>
+      <c r="BK53" s="1">
+        <v>1.042841899E-3</v>
+      </c>
     </row>
-    <row r="54" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>10.4</v>
       </c>
@@ -10401,8 +10887,17 @@
       <c r="BH54" s="1">
         <v>5.029625601E-3</v>
       </c>
+      <c r="BI54" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="BJ54" s="1">
+        <v>7.9735182260000006E-3</v>
+      </c>
+      <c r="BK54" s="1">
+        <v>1.244226758E-3</v>
+      </c>
     </row>
-    <row r="55" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>10.6</v>
       </c>
@@ -10583,8 +11078,17 @@
       <c r="BH55" s="1">
         <v>6.8113177629999999E-3</v>
       </c>
+      <c r="BI55" s="1">
+        <v>10.6</v>
+      </c>
+      <c r="BJ55" s="1">
+        <v>6.3654064940000003E-3</v>
+      </c>
+      <c r="BK55" s="1">
+        <v>-2.0357291380000001E-4</v>
+      </c>
     </row>
-    <row r="56" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>10.8</v>
       </c>
@@ -10765,8 +11269,17 @@
       <c r="BH56" s="1">
         <v>5.5925697060000001E-3</v>
       </c>
+      <c r="BI56" s="1">
+        <v>10.8</v>
+      </c>
+      <c r="BJ56" s="1">
+        <v>6.7836260479999999E-3</v>
+      </c>
+      <c r="BK56" s="1">
+        <v>-1.1505583300000001E-3</v>
+      </c>
     </row>
-    <row r="57" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>11</v>
       </c>
@@ -10947,8 +11460,17 @@
       <c r="BH57" s="1">
         <v>4.1621741550000001E-3</v>
       </c>
+      <c r="BI57" s="1">
+        <v>11</v>
+      </c>
+      <c r="BJ57" s="1">
+        <v>7.5078958159999999E-3</v>
+      </c>
+      <c r="BK57" s="1">
+        <v>-6.6626969049999999E-4</v>
+      </c>
     </row>
-    <row r="58" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>11.2</v>
       </c>
@@ -11129,8 +11651,17 @@
       <c r="BH58" s="1">
         <v>4.5200246209999998E-3</v>
       </c>
+      <c r="BI58" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="BJ58" s="1">
+        <v>8.6536419109999995E-3</v>
+      </c>
+      <c r="BK58" s="1">
+        <v>-1.157159276E-3</v>
+      </c>
     </row>
-    <row r="59" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>11.4</v>
       </c>
@@ -11311,8 +11842,17 @@
       <c r="BH59" s="1">
         <v>4.2980907230000002E-3</v>
       </c>
+      <c r="BI59" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="BJ59" s="1">
+        <v>8.7072045649999995E-3</v>
+      </c>
+      <c r="BK59" s="1">
+        <v>-1.1698940110000001E-3</v>
+      </c>
     </row>
-    <row r="60" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>11.6</v>
       </c>
@@ -11493,8 +12033,17 @@
       <c r="BH60" s="1">
         <v>3.4096304790000001E-3</v>
       </c>
+      <c r="BI60" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="BJ60" s="1">
+        <v>8.1466963619999996E-3</v>
+      </c>
+      <c r="BK60" s="1">
+        <v>-1.2684580359999999E-3</v>
+      </c>
     </row>
-    <row r="61" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>11.8</v>
       </c>
@@ -11675,8 +12224,17 @@
       <c r="BH61" s="1">
         <v>2.5497274549999998E-3</v>
       </c>
+      <c r="BI61" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="BJ61" s="1">
+        <v>6.8187277799999996E-3</v>
+      </c>
+      <c r="BK61" s="1">
+        <v>-7.2644643589999996E-4</v>
+      </c>
     </row>
-    <row r="62" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>12</v>
       </c>
@@ -11857,8 +12415,17 @@
       <c r="BH62" s="1">
         <v>2.1199390450000002E-3</v>
       </c>
+      <c r="BI62" s="1">
+        <v>12</v>
+      </c>
+      <c r="BJ62" s="1">
+        <v>5.7984779560000003E-3</v>
+      </c>
+      <c r="BK62" s="1">
+        <v>-1.5405285029999999E-3</v>
+      </c>
     </row>
-    <row r="63" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>12.2</v>
       </c>
@@ -12039,8 +12606,17 @@
       <c r="BH63" s="1">
         <v>3.9482402769999998E-3</v>
       </c>
+      <c r="BI63" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="BJ63" s="1">
+        <v>5.7499660289999999E-3</v>
+      </c>
+      <c r="BK63" s="1">
+        <v>-1.2648884679999999E-3</v>
+      </c>
     </row>
-    <row r="64" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>12.4</v>
       </c>
@@ -12221,8 +12797,17 @@
       <c r="BH64" s="1">
         <v>3.7434598780000002E-3</v>
       </c>
+      <c r="BI64" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="BJ64" s="1">
+        <v>6.1505032259999998E-3</v>
+      </c>
+      <c r="BK64" s="1">
+        <v>-6.4061180439999997E-4</v>
+      </c>
     </row>
-    <row r="65" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>12.6</v>
       </c>
@@ -12403,8 +12988,17 @@
       <c r="BH65" s="1">
         <v>3.6982679929999998E-3</v>
       </c>
+      <c r="BI65" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="BJ65" s="1">
+        <v>6.3565532470000003E-3</v>
+      </c>
+      <c r="BK65" s="1">
+        <v>1.2827081859999999E-3</v>
+      </c>
     </row>
-    <row r="66" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>12.8</v>
       </c>
@@ -12585,8 +13179,17 @@
       <c r="BH66" s="1">
         <v>3.3411290409999998E-3</v>
       </c>
+      <c r="BI66" s="1">
+        <v>12.8</v>
+      </c>
+      <c r="BJ66" s="1">
+        <v>6.5953610390000004E-3</v>
+      </c>
+      <c r="BK66" s="1">
+        <v>2.5430024589999998E-3</v>
+      </c>
     </row>
-    <row r="67" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>13</v>
       </c>
@@ -12767,8 +13370,17 @@
       <c r="BH67" s="1">
         <v>2.8612396570000002E-3</v>
       </c>
+      <c r="BI67" s="1">
+        <v>13</v>
+      </c>
+      <c r="BJ67" s="1">
+        <v>7.2874735800000003E-3</v>
+      </c>
+      <c r="BK67" s="1">
+        <v>3.3479937019999999E-3</v>
+      </c>
     </row>
-    <row r="68" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>13.2</v>
       </c>
@@ -12949,8 +13561,17 @@
       <c r="BH68" s="1">
         <v>2.4387622260000001E-3</v>
       </c>
+      <c r="BI68" s="1">
+        <v>13.2</v>
+      </c>
+      <c r="BJ68" s="1">
+        <v>7.2848508939999997E-3</v>
+      </c>
+      <c r="BK68" s="1">
+        <v>4.2825734050000001E-3</v>
+      </c>
     </row>
-    <row r="69" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>13.4</v>
       </c>
@@ -13131,8 +13752,17 @@
       <c r="BH69" s="1">
         <v>2.7851354730000001E-3</v>
       </c>
+      <c r="BI69" s="1">
+        <v>13.4</v>
+      </c>
+      <c r="BJ69" s="1">
+        <v>7.5783555590000001E-3</v>
+      </c>
+      <c r="BK69" s="1">
+        <v>3.861264032E-3</v>
+      </c>
     </row>
-    <row r="70" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>13.6</v>
       </c>
@@ -13313,8 +13943,17 @@
       <c r="BH70" s="1">
         <v>2.8163359530000002E-3</v>
       </c>
+      <c r="BI70" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="BJ70" s="1">
+        <v>7.283394076E-3</v>
+      </c>
+      <c r="BK70" s="1">
+        <v>3.4874710180000002E-3</v>
+      </c>
     </row>
-    <row r="71" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>13.8</v>
       </c>
@@ -13495,8 +14134,17 @@
       <c r="BH71" s="1">
         <v>3.4480511250000001E-3</v>
       </c>
+      <c r="BI71" s="1">
+        <v>13.8</v>
+      </c>
+      <c r="BJ71" s="1">
+        <v>7.7407235369999997E-3</v>
+      </c>
+      <c r="BK71" s="1">
+        <v>3.0638226020000001E-3</v>
+      </c>
     </row>
-    <row r="72" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>14</v>
       </c>
@@ -13677,8 +14325,17 @@
       <c r="BH72" s="1">
         <v>5.4528109039999996E-3</v>
       </c>
+      <c r="BI72" s="1">
+        <v>14</v>
+      </c>
+      <c r="BJ72" s="1">
+        <v>7.9679573799999997E-3</v>
+      </c>
+      <c r="BK72" s="1">
+        <v>3.788579172E-3</v>
+      </c>
     </row>
-    <row r="73" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>14.2</v>
       </c>
@@ -13859,8 +14516,17 @@
       <c r="BH73" s="1">
         <v>4.8695356400000004E-3</v>
       </c>
+      <c r="BI73" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="BJ73" s="1">
+        <v>7.1038827129999999E-3</v>
+      </c>
+      <c r="BK73" s="1">
+        <v>3.390212573E-3</v>
+      </c>
     </row>
-    <row r="74" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>14.4</v>
       </c>
@@ -14041,8 +14707,17 @@
       <c r="BH74" s="1">
         <v>4.1071707950000001E-3</v>
       </c>
+      <c r="BI74" s="1">
+        <v>14.4</v>
+      </c>
+      <c r="BJ74" s="1">
+        <v>6.7125509850000003E-3</v>
+      </c>
+      <c r="BK74" s="1">
+        <v>2.0144478240000001E-3</v>
+      </c>
     </row>
-    <row r="75" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>14.6</v>
       </c>
@@ -14223,8 +14898,17 @@
       <c r="BH75" s="1">
         <v>3.5136025500000002E-3</v>
       </c>
+      <c r="BI75" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="BJ75" s="1">
+        <v>5.4078737910000004E-3</v>
+      </c>
+      <c r="BK75" s="1">
+        <v>2.6707876310000001E-3</v>
+      </c>
     </row>
-    <row r="76" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>14.8</v>
       </c>
@@ -14405,8 +15089,17 @@
       <c r="BH76" s="1">
         <v>2.35720646E-3</v>
       </c>
+      <c r="BI76" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="BJ76" s="1">
+        <v>5.5781911160000001E-3</v>
+      </c>
+      <c r="BK76" s="1">
+        <v>2.320316378E-3</v>
+      </c>
     </row>
-    <row r="77" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>15</v>
       </c>
@@ -14587,8 +15280,17 @@
       <c r="BH77" s="1">
         <v>3.6215894099999998E-3</v>
       </c>
+      <c r="BI77" s="1">
+        <v>15</v>
+      </c>
+      <c r="BJ77" s="1">
+        <v>5.6764865200000002E-3</v>
+      </c>
+      <c r="BK77" s="1">
+        <v>2.4143884759999999E-4</v>
+      </c>
     </row>
-    <row r="78" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>15.2</v>
       </c>
@@ -14769,8 +15471,17 @@
       <c r="BH78" s="1">
         <v>3.9642033710000002E-3</v>
       </c>
+      <c r="BI78" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="BJ78" s="1">
+        <v>5.0583950289999997E-3</v>
+      </c>
+      <c r="BK78" s="1">
+        <v>1.089005023E-3</v>
+      </c>
     </row>
-    <row r="79" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>15.4</v>
       </c>
@@ -14951,8 +15662,17 @@
       <c r="BH79" s="1">
         <v>3.6148603879999999E-3</v>
       </c>
+      <c r="BI79" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="BJ79" s="1">
+        <v>3.343281765E-3</v>
+      </c>
+      <c r="BK79" s="1">
+        <v>6.5203780419999995E-4</v>
+      </c>
     </row>
-    <row r="80" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>15.6</v>
       </c>
@@ -15133,8 +15853,17 @@
       <c r="BH80" s="1">
         <v>4.7916386300000001E-3</v>
       </c>
+      <c r="BI80" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="BJ80" s="1">
+        <v>2.4802692430000001E-3</v>
+      </c>
+      <c r="BK80" s="1">
+        <v>5.4526290540000001E-4</v>
+      </c>
     </row>
-    <row r="81" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>15.8</v>
       </c>
@@ -15315,8 +16044,17 @@
       <c r="BH81" s="1">
         <v>6.5748168390000004E-3</v>
       </c>
+      <c r="BI81" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="BJ81" s="1">
+        <v>3.5697780429999998E-3</v>
+      </c>
+      <c r="BK81" s="1">
+        <v>-9.0250855670000001E-4</v>
+      </c>
     </row>
-    <row r="82" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>16</v>
       </c>
@@ -15497,8 +16235,17 @@
       <c r="BH82" s="1">
         <v>7.2445770899999999E-3</v>
       </c>
+      <c r="BI82" s="1">
+        <v>16</v>
+      </c>
+      <c r="BJ82" s="1">
+        <v>4.0959348899999998E-3</v>
+      </c>
+      <c r="BK82" s="1">
+        <v>-1.4783745029999999E-3</v>
+      </c>
     </row>
-    <row r="83" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>16.2</v>
       </c>
@@ -15679,8 +16426,17 @@
       <c r="BH83" s="1">
         <v>6.7931720919999997E-3</v>
       </c>
+      <c r="BI83" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="BJ83" s="1">
+        <v>3.9162361820000002E-3</v>
+      </c>
+      <c r="BK83" s="1">
+        <v>-1.062473275E-3</v>
+      </c>
     </row>
-    <row r="84" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>16.399999999999999</v>
       </c>
@@ -15861,8 +16617,17 @@
       <c r="BH84" s="1">
         <v>8.0093950769999991E-3</v>
       </c>
+      <c r="BI84" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="BJ84" s="1">
+        <v>3.801068291E-3</v>
+      </c>
+      <c r="BK84" s="1">
+        <v>-1.7578262770000001E-3</v>
+      </c>
     </row>
-    <row r="85" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>16.600000000000001</v>
       </c>
@@ -16043,8 +16808,17 @@
       <c r="BH85" s="1">
         <v>8.7424299119999993E-3</v>
       </c>
+      <c r="BI85" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="BJ85" s="1">
+        <v>3.4562966149999999E-3</v>
+      </c>
+      <c r="BK85" s="1">
+        <v>-2.2172500469999998E-3</v>
+      </c>
     </row>
-    <row r="86" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>16.8</v>
       </c>
@@ -16225,8 +16999,17 @@
       <c r="BH86" s="1">
         <v>8.4055755549999993E-3</v>
       </c>
+      <c r="BI86" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="BJ86" s="1">
+        <v>3.5748697969999999E-3</v>
+      </c>
+      <c r="BK86" s="1">
+        <v>-2.332725526E-3</v>
+      </c>
     </row>
-    <row r="87" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>17</v>
       </c>
@@ -16407,8 +17190,17 @@
       <c r="BH87" s="1">
         <v>8.5764609859999997E-3</v>
       </c>
+      <c r="BI87" s="1">
+        <v>17</v>
+      </c>
+      <c r="BJ87" s="1">
+        <v>2.1427497579999998E-3</v>
+      </c>
+      <c r="BK87" s="1">
+        <v>-1.930200979E-3</v>
+      </c>
     </row>
-    <row r="88" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>17.2</v>
       </c>
@@ -16589,8 +17381,17 @@
       <c r="BH88" s="1">
         <v>9.1474855639999998E-3</v>
       </c>
+      <c r="BI88" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="BJ88" s="1">
+        <v>1.5830652949999999E-3</v>
+      </c>
+      <c r="BK88" s="1">
+        <v>-1.6752414169999999E-3</v>
+      </c>
     </row>
-    <row r="89" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>17.399999999999999</v>
       </c>
@@ -16771,8 +17572,17 @@
       <c r="BH89" s="1">
         <v>9.0271162600000007E-3</v>
       </c>
+      <c r="BI89" s="1">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="BJ89" s="1">
+        <v>1.9746358239999999E-3</v>
+      </c>
+      <c r="BK89" s="1">
+        <v>-1.6408553179999999E-3</v>
+      </c>
     </row>
-    <row r="90" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>17.600000000000001</v>
       </c>
@@ -16953,8 +17763,17 @@
       <c r="BH90" s="1">
         <v>9.7518557609999994E-3</v>
       </c>
+      <c r="BI90" s="1">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="BJ90" s="1">
+        <v>1.519013618E-3</v>
+      </c>
+      <c r="BK90" s="1">
+        <v>-3.4177324839999999E-3</v>
+      </c>
     </row>
-    <row r="91" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>17.8</v>
       </c>
@@ -17135,8 +17954,17 @@
       <c r="BH91" s="1">
         <v>1.0064633850000001E-2</v>
       </c>
+      <c r="BI91" s="1">
+        <v>17.8</v>
+      </c>
+      <c r="BJ91" s="1">
+        <v>3.6946894460000002E-4</v>
+      </c>
+      <c r="BK91" s="1">
+        <v>-3.9035913080000002E-3</v>
+      </c>
     </row>
-    <row r="92" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>18</v>
       </c>
@@ -17317,8 +18145,17 @@
       <c r="BH92" s="1">
         <v>9.8415539859999998E-3</v>
       </c>
+      <c r="BI92" s="1">
+        <v>18</v>
+      </c>
+      <c r="BJ92" s="1">
+        <v>1.1168736900000001E-3</v>
+      </c>
+      <c r="BK92" s="1">
+        <v>-2.37457051E-3</v>
+      </c>
     </row>
-    <row r="93" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>18.2</v>
       </c>
@@ -17499,8 +18336,17 @@
       <c r="BH93" s="1">
         <v>1.0847843940000001E-2</v>
       </c>
+      <c r="BI93" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="BJ93" s="1">
+        <v>2.5481009629999998E-3</v>
+      </c>
+      <c r="BK93" s="1">
+        <v>-2.9673819910000002E-3</v>
+      </c>
     </row>
-    <row r="94" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>18.399999999999999</v>
       </c>
@@ -17681,8 +18527,17 @@
       <c r="BH94" s="1">
         <v>1.085259234E-2</v>
       </c>
+      <c r="BI94" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="BJ94" s="1">
+        <v>1.5159813549999999E-3</v>
+      </c>
+      <c r="BK94" s="1">
+        <v>-2.439255541E-3</v>
+      </c>
     </row>
-    <row r="95" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>18.600000000000001</v>
       </c>
@@ -17863,8 +18718,17 @@
       <c r="BH95" s="1">
         <v>1.0377272789999999E-2</v>
       </c>
+      <c r="BI95" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="BJ95" s="1">
+        <v>3.1704685989999998E-3</v>
+      </c>
+      <c r="BK95" s="1">
+        <v>-3.0056986710000001E-3</v>
+      </c>
     </row>
-    <row r="96" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>18.8</v>
       </c>
@@ -18045,8 +18909,17 @@
       <c r="BH96" s="1">
         <v>8.0711437669999993E-3</v>
       </c>
+      <c r="BI96" s="1">
+        <v>18.8</v>
+      </c>
+      <c r="BJ96" s="1">
+        <v>3.2897428270000002E-3</v>
+      </c>
+      <c r="BK96" s="1">
+        <v>-2.5066321329999999E-3</v>
+      </c>
     </row>
-    <row r="97" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>19</v>
       </c>
@@ -18227,8 +19100,17 @@
       <c r="BH97" s="1">
         <v>7.4687777210000004E-3</v>
       </c>
+      <c r="BI97" s="1">
+        <v>19</v>
+      </c>
+      <c r="BJ97" s="1">
+        <v>4.7681688010000004E-3</v>
+      </c>
+      <c r="BK97" s="1">
+        <v>-1.4107649890000001E-3</v>
+      </c>
     </row>
-    <row r="98" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>19.2</v>
       </c>
@@ -18409,8 +19291,17 @@
       <c r="BH98" s="1">
         <v>8.1409862749999996E-3</v>
       </c>
+      <c r="BI98" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="BJ98" s="1">
+        <v>4.8259003370000001E-3</v>
+      </c>
+      <c r="BK98" s="1">
+        <v>-1.6060949909999999E-3</v>
+      </c>
     </row>
-    <row r="99" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>19.399999999999999</v>
       </c>
@@ -18591,8 +19482,17 @@
       <c r="BH99" s="1">
         <v>8.4460922130000001E-3</v>
       </c>
+      <c r="BI99" s="1">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="BJ99" s="1">
+        <v>6.0261788000000004E-3</v>
+      </c>
+      <c r="BK99" s="1">
+        <v>-1.3549450149999999E-3</v>
+      </c>
     </row>
-    <row r="100" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>19.600000000000001</v>
       </c>
@@ -18773,8 +19673,17 @@
       <c r="BH100" s="1">
         <v>6.8587020400000002E-3</v>
       </c>
+      <c r="BI100" s="1">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="BJ100" s="1">
+        <v>5.8613068789999997E-3</v>
+      </c>
+      <c r="BK100" s="1">
+        <v>-2.1842690830000001E-3</v>
+      </c>
     </row>
-    <row r="101" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>19.8</v>
       </c>
@@ -18955,8 +19864,17 @@
       <c r="BH101" s="1">
         <v>7.0566615089999998E-3</v>
       </c>
+      <c r="BI101" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="BJ101" s="1">
+        <v>5.4025626450000001E-3</v>
+      </c>
+      <c r="BK101" s="1">
+        <v>-3.6980094469999999E-3</v>
+      </c>
     </row>
-    <row r="102" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>20</v>
       </c>
@@ -19137,8 +20055,17 @@
       <c r="BH102" s="1">
         <v>8.7094695419999996E-3</v>
       </c>
+      <c r="BI102" s="1">
+        <v>20</v>
+      </c>
+      <c r="BJ102" s="1">
+        <v>4.7135861739999998E-3</v>
+      </c>
+      <c r="BK102" s="1">
+        <v>-1.506971491E-3</v>
+      </c>
     </row>
-    <row r="103" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>20.2</v>
       </c>
@@ -19319,8 +20246,17 @@
       <c r="BH103" s="1">
         <v>9.9212003530000006E-3</v>
       </c>
+      <c r="BI103" s="1">
+        <v>20.2</v>
+      </c>
+      <c r="BJ103" s="1">
+        <v>6.4316260429999996E-3</v>
+      </c>
+      <c r="BK103" s="1">
+        <v>-2.1808302750000001E-3</v>
+      </c>
     </row>
-    <row r="104" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>20.399999999999999</v>
       </c>
@@ -19501,8 +20437,17 @@
       <c r="BH104" s="1">
         <v>8.2810885800000001E-3</v>
       </c>
+      <c r="BI104" s="1">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="BJ104" s="1">
+        <v>6.2579545830000003E-3</v>
+      </c>
+      <c r="BK104" s="1">
+        <v>-2.4638909789999998E-3</v>
+      </c>
     </row>
-    <row r="105" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>20.6</v>
       </c>
@@ -19683,8 +20628,17 @@
       <c r="BH105" s="1">
         <v>7.9109210830000005E-3</v>
       </c>
+      <c r="BI105" s="1">
+        <v>20.6</v>
+      </c>
+      <c r="BJ105" s="1">
+        <v>4.2595712040000002E-3</v>
+      </c>
+      <c r="BK105" s="1">
+        <v>-2.6260800029999998E-3</v>
+      </c>
     </row>
-    <row r="106" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>20.8</v>
       </c>
@@ -19865,8 +20819,17 @@
       <c r="BH106" s="1">
         <v>7.9089557750000004E-3</v>
       </c>
+      <c r="BI106" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="BJ106" s="1">
+        <v>4.8366498849999997E-3</v>
+      </c>
+      <c r="BK106" s="1">
+        <v>-2.1893806569999999E-3</v>
+      </c>
     </row>
-    <row r="107" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>21</v>
       </c>
@@ -20047,8 +21010,17 @@
       <c r="BH107" s="1">
         <v>7.6787661649999998E-3</v>
       </c>
+      <c r="BI107" s="1">
+        <v>21</v>
+      </c>
+      <c r="BJ107" s="1">
+        <v>4.5497652419999998E-3</v>
+      </c>
+      <c r="BK107" s="1">
+        <v>-2.174023811E-3</v>
+      </c>
     </row>
-    <row r="108" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>21.2</v>
       </c>
@@ -20229,8 +21201,17 @@
       <c r="BH108" s="1">
         <v>7.0742600829999999E-3</v>
       </c>
+      <c r="BI108" s="1">
+        <v>21.2</v>
+      </c>
+      <c r="BJ108" s="1">
+        <v>4.6067322399999996E-3</v>
+      </c>
+      <c r="BK108" s="1">
+        <v>-1.785389394E-3</v>
+      </c>
     </row>
-    <row r="109" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>21.4</v>
       </c>
@@ -20411,8 +21392,17 @@
       <c r="BH109" s="1">
         <v>9.1268621310000003E-3</v>
       </c>
+      <c r="BI109" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="BJ109" s="1">
+        <v>4.8280119450000002E-3</v>
+      </c>
+      <c r="BK109" s="1">
+        <v>-1.6524865289999999E-3</v>
+      </c>
     </row>
-    <row r="110" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>21.6</v>
       </c>
@@ -20593,8 +21583,17 @@
       <c r="BH110" s="1">
         <v>9.2666119550000002E-3</v>
       </c>
+      <c r="BI110" s="1">
+        <v>21.6</v>
+      </c>
+      <c r="BJ110" s="1">
+        <v>6.1940191699999996E-3</v>
+      </c>
+      <c r="BK110" s="1">
+        <v>-1.73563835E-3</v>
+      </c>
     </row>
-    <row r="111" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>21.8</v>
       </c>
@@ -20775,8 +21774,17 @@
       <c r="BH111" s="1">
         <v>9.5229043819999998E-3</v>
       </c>
+      <c r="BI111" s="1">
+        <v>21.8</v>
+      </c>
+      <c r="BJ111" s="1">
+        <v>6.6043091050000001E-3</v>
+      </c>
+      <c r="BK111" s="1">
+        <v>-2.4628422969999999E-3</v>
+      </c>
     </row>
-    <row r="112" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>22</v>
       </c>
@@ -20957,8 +21965,17 @@
       <c r="BH112" s="1">
         <v>1.1126314409999999E-2</v>
       </c>
+      <c r="BI112" s="1">
+        <v>22</v>
+      </c>
+      <c r="BJ112" s="1">
+        <v>6.3184680510000001E-3</v>
+      </c>
+      <c r="BK112" s="1">
+        <v>-2.6463270770000001E-3</v>
+      </c>
     </row>
-    <row r="113" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>22.2</v>
       </c>
@@ -21139,8 +22156,17 @@
       <c r="BH113" s="1">
         <v>1.2550487609999999E-2</v>
       </c>
+      <c r="BI113" s="1">
+        <v>22.2</v>
+      </c>
+      <c r="BJ113" s="1">
+        <v>6.1411198439999997E-3</v>
+      </c>
+      <c r="BK113" s="1">
+        <v>-1.2600838799999999E-3</v>
+      </c>
     </row>
-    <row r="114" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>22.4</v>
       </c>
@@ -21321,8 +22347,17 @@
       <c r="BH114" s="1">
         <v>1.195165772E-2</v>
       </c>
+      <c r="BI114" s="1">
+        <v>22.4</v>
+      </c>
+      <c r="BJ114" s="1">
+        <v>6.3707720340000001E-3</v>
+      </c>
+      <c r="BK114" s="1">
+        <v>-1.5812601049999999E-3</v>
+      </c>
     </row>
-    <row r="115" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>22.6</v>
       </c>
@@ -21503,8 +22538,17 @@
       <c r="BH115" s="1">
         <v>1.22213711E-2</v>
       </c>
+      <c r="BI115" s="1">
+        <v>22.6</v>
+      </c>
+      <c r="BJ115" s="1">
+        <v>6.4152343289999997E-3</v>
+      </c>
+      <c r="BK115" s="1">
+        <v>-1.510525913E-3</v>
+      </c>
     </row>
-    <row r="116" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>22.8</v>
       </c>
@@ -21685,8 +22729,17 @@
       <c r="BH116" s="1">
         <v>1.087232411E-2</v>
       </c>
+      <c r="BI116" s="1">
+        <v>22.8</v>
+      </c>
+      <c r="BJ116" s="1">
+        <v>5.290482002E-3</v>
+      </c>
+      <c r="BK116" s="1">
+        <v>-1.2015908809999999E-3</v>
+      </c>
     </row>
-    <row r="117" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>23</v>
       </c>
@@ -21867,8 +22920,17 @@
       <c r="BH117" s="1">
         <v>9.1207187110000001E-3</v>
       </c>
+      <c r="BI117" s="1">
+        <v>23</v>
+      </c>
+      <c r="BJ117" s="1">
+        <v>3.6335444199999999E-3</v>
+      </c>
+      <c r="BK117" s="1">
+        <v>-1.2100632749999999E-3</v>
+      </c>
     </row>
-    <row r="118" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>23.2</v>
       </c>
@@ -22049,8 +23111,17 @@
       <c r="BH118" s="1">
         <v>9.2279541679999993E-3</v>
       </c>
+      <c r="BI118" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="BJ118" s="1">
+        <v>3.0039648069999998E-3</v>
+      </c>
+      <c r="BK118" s="1">
+        <v>-2.1563256690000001E-3</v>
+      </c>
     </row>
-    <row r="119" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>23.4</v>
       </c>
@@ -22231,8 +23302,17 @@
       <c r="BH119" s="1">
         <v>1.0091186110000001E-2</v>
       </c>
+      <c r="BI119" s="1">
+        <v>23.4</v>
+      </c>
+      <c r="BJ119" s="1">
+        <v>1.1217930520000001E-3</v>
+      </c>
+      <c r="BK119" s="1">
+        <v>-4.1139100249999996E-3</v>
+      </c>
     </row>
-    <row r="120" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>23.6</v>
       </c>
@@ -22413,8 +23493,17 @@
       <c r="BH120" s="1">
         <v>1.11402177E-2</v>
       </c>
+      <c r="BI120" s="1">
+        <v>23.6</v>
+      </c>
+      <c r="BJ120" s="1">
+        <v>4.3435410549999998E-4</v>
+      </c>
+      <c r="BK120" s="1">
+        <v>-3.404088981E-3</v>
+      </c>
     </row>
-    <row r="121" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>23.8</v>
       </c>
@@ -22595,8 +23684,17 @@
       <c r="BH121" s="1">
         <v>1.074909366E-2</v>
       </c>
+      <c r="BI121" s="1">
+        <v>23.8</v>
+      </c>
+      <c r="BJ121" s="1">
+        <v>1.117904031E-3</v>
+      </c>
+      <c r="BK121" s="1">
+        <v>-4.4902827849999999E-3</v>
+      </c>
     </row>
-    <row r="122" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>24</v>
       </c>
@@ -22777,8 +23875,17 @@
       <c r="BH122" s="1">
         <v>1.306461691E-2</v>
       </c>
+      <c r="BI122" s="1">
+        <v>24</v>
+      </c>
+      <c r="BJ122" s="1">
+        <v>1.2176742299999999E-3</v>
+      </c>
+      <c r="BK122" s="1">
+        <v>-4.7628106999999999E-3</v>
+      </c>
     </row>
-    <row r="123" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>24.2</v>
       </c>
@@ -22959,8 +24066,17 @@
       <c r="BH123" s="1">
         <v>1.203521728E-2</v>
       </c>
+      <c r="BI123" s="1">
+        <v>24.2</v>
+      </c>
+      <c r="BJ123" s="1">
+        <v>1.6912790099999999E-3</v>
+      </c>
+      <c r="BK123" s="1">
+        <v>-4.7901347469999998E-3</v>
+      </c>
     </row>
-    <row r="124" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>24.4</v>
       </c>
@@ -23141,8 +24257,17 @@
       <c r="BH124" s="1">
         <v>1.1668618889999999E-2</v>
       </c>
+      <c r="BI124" s="1">
+        <v>24.4</v>
+      </c>
+      <c r="BJ124" s="1">
+        <v>3.8041399699999999E-4</v>
+      </c>
+      <c r="BK124" s="1">
+        <v>-5.8714156410000001E-3</v>
+      </c>
     </row>
-    <row r="125" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>24.6</v>
       </c>
@@ -23323,8 +24448,17 @@
       <c r="BH125" s="1">
         <v>1.4176439759999999E-2</v>
       </c>
+      <c r="BI125" s="1">
+        <v>24.6</v>
+      </c>
+      <c r="BJ125" s="1">
+        <v>5.5501208519999996E-4</v>
+      </c>
+      <c r="BK125" s="1">
+        <v>-4.920638156E-3</v>
+      </c>
     </row>
-    <row r="126" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>24.8</v>
       </c>
@@ -23505,8 +24639,17 @@
       <c r="BH126" s="1">
         <v>1.5873484909999999E-2</v>
       </c>
+      <c r="BI126" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="BJ126" s="1">
+        <v>-7.6303686550000002E-5</v>
+      </c>
+      <c r="BK126" s="1">
+        <v>-4.7407004150000001E-3</v>
+      </c>
     </row>
-    <row r="127" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>25</v>
       </c>
@@ -23687,8 +24830,17 @@
       <c r="BH127" s="1">
         <v>1.5680282930000001E-2</v>
       </c>
+      <c r="BI127" s="1">
+        <v>25</v>
+      </c>
+      <c r="BJ127" s="1">
+        <v>-1.8558967019999999E-3</v>
+      </c>
+      <c r="BK127" s="1">
+        <v>-5.1699716439999998E-3</v>
+      </c>
     </row>
-    <row r="128" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>25.2</v>
       </c>
@@ -23869,8 +25021,17 @@
       <c r="BH128" s="1">
         <v>1.6166564080000001E-2</v>
       </c>
+      <c r="BI128" s="1">
+        <v>25.2</v>
+      </c>
+      <c r="BJ128" s="1">
+        <v>-2.416239687E-3</v>
+      </c>
+      <c r="BK128" s="1">
+        <v>-4.5114024449999998E-3</v>
+      </c>
     </row>
-    <row r="129" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>25.4</v>
       </c>
@@ -24051,8 +25212,17 @@
       <c r="BH129" s="1">
         <v>1.5413773130000001E-2</v>
       </c>
+      <c r="BI129" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="BJ129" s="1">
+        <v>-2.1340187249999998E-3</v>
+      </c>
+      <c r="BK129" s="1">
+        <v>-4.4996094950000001E-3</v>
+      </c>
     </row>
-    <row r="130" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>25.6</v>
       </c>
@@ -24233,8 +25403,17 @@
       <c r="BH130" s="1">
         <v>1.5583339349999999E-2</v>
       </c>
+      <c r="BI130" s="1">
+        <v>25.6</v>
+      </c>
+      <c r="BJ130" s="1">
+        <v>-4.1871761189999999E-3</v>
+      </c>
+      <c r="BK130" s="1">
+        <v>-4.0459604059999996E-3</v>
+      </c>
     </row>
-    <row r="131" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>25.8</v>
       </c>
@@ -24415,8 +25594,17 @@
       <c r="BH131" s="1">
         <v>1.589585651E-2</v>
       </c>
+      <c r="BI131" s="1">
+        <v>25.8</v>
+      </c>
+      <c r="BJ131" s="1">
+        <v>-6.1342949129999996E-3</v>
+      </c>
+      <c r="BK131" s="1">
+        <v>-3.803149978E-3</v>
+      </c>
     </row>
-    <row r="132" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>26</v>
       </c>
@@ -24597,8 +25785,17 @@
       <c r="BH132" s="1">
         <v>1.6495749050000001E-2</v>
       </c>
+      <c r="BI132" s="1">
+        <v>26</v>
+      </c>
+      <c r="BJ132" s="1">
+        <v>-5.7274442690000002E-3</v>
+      </c>
+      <c r="BK132" s="1">
+        <v>-3.6972106630000002E-3</v>
+      </c>
     </row>
-    <row r="133" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>26.2</v>
       </c>
@@ -24779,8 +25976,17 @@
       <c r="BH133" s="1">
         <v>1.718958395E-2</v>
       </c>
+      <c r="BI133" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="BJ133" s="1">
+        <v>-5.1555565670000003E-3</v>
+      </c>
+      <c r="BK133" s="1">
+        <v>-4.564986006E-3</v>
+      </c>
     </row>
-    <row r="134" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>26.4</v>
       </c>
@@ -24961,8 +26167,17 @@
       <c r="BH134" s="1">
         <v>1.6809503529999999E-2</v>
       </c>
+      <c r="BI134" s="1">
+        <v>26.4</v>
+      </c>
+      <c r="BJ134" s="1">
+        <v>-3.7942069380000002E-3</v>
+      </c>
+      <c r="BK134" s="1">
+        <v>-2.7663392799999998E-3</v>
+      </c>
     </row>
-    <row r="135" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>26.6</v>
       </c>
@@ -25143,8 +26358,17 @@
       <c r="BH135" s="1">
         <v>1.519936061E-2</v>
       </c>
+      <c r="BI135" s="1">
+        <v>26.6</v>
+      </c>
+      <c r="BJ135" s="1">
+        <v>-2.4603414739999998E-3</v>
+      </c>
+      <c r="BK135" s="1">
+        <v>-2.3529874419999999E-3</v>
+      </c>
     </row>
-    <row r="136" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>26.8</v>
       </c>
@@ -25325,8 +26549,17 @@
       <c r="BH136" s="1">
         <v>1.4353358429999999E-2</v>
       </c>
+      <c r="BI136" s="1">
+        <v>26.8</v>
+      </c>
+      <c r="BJ136" s="1">
+        <v>-2.1234650270000001E-3</v>
+      </c>
+      <c r="BK136" s="1">
+        <v>-2.4641783980000002E-3</v>
+      </c>
     </row>
-    <row r="137" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>27</v>
       </c>
@@ -25507,8 +26740,17 @@
       <c r="BH137" s="1">
         <v>1.4813876070000001E-2</v>
       </c>
+      <c r="BI137" s="1">
+        <v>27</v>
+      </c>
+      <c r="BJ137" s="1">
+        <v>-1.554476193E-3</v>
+      </c>
+      <c r="BK137" s="1">
+        <v>-2.751432833E-3</v>
+      </c>
     </row>
-    <row r="138" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>27.2</v>
       </c>
@@ -25689,8 +26931,17 @@
       <c r="BH138" s="1">
         <v>1.6264636919999999E-2</v>
       </c>
+      <c r="BI138" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="BJ138" s="1">
+        <v>-2.3561211669999998E-3</v>
+      </c>
+      <c r="BK138" s="1">
+        <v>-2.6844238580000001E-3</v>
+      </c>
     </row>
-    <row r="139" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>27.4</v>
       </c>
@@ -25871,8 +27122,17 @@
       <c r="BH139" s="1">
         <v>1.681273183E-2</v>
       </c>
+      <c r="BI139" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="BJ139" s="1">
+        <v>-1.562144089E-3</v>
+      </c>
+      <c r="BK139" s="1">
+        <v>-3.0159192060000002E-3</v>
+      </c>
     </row>
-    <row r="140" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>27.6</v>
       </c>
@@ -26053,8 +27313,17 @@
       <c r="BH140" s="1">
         <v>1.8279321929999998E-2</v>
       </c>
+      <c r="BI140" s="1">
+        <v>27.6</v>
+      </c>
+      <c r="BJ140" s="1">
+        <v>-1.445052334E-3</v>
+      </c>
+      <c r="BK140" s="1">
+        <v>-2.8166047659999999E-3</v>
+      </c>
     </row>
-    <row r="141" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>27.8</v>
       </c>
@@ -26235,8 +27504,17 @@
       <c r="BH141" s="1">
         <v>1.8825193340000001E-2</v>
       </c>
+      <c r="BI141" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="BJ141" s="1">
+        <v>-2.3613196470000002E-3</v>
+      </c>
+      <c r="BK141" s="1">
+        <v>-3.9200537240000003E-3</v>
+      </c>
     </row>
-    <row r="142" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>28</v>
       </c>
@@ -26417,8 +27695,17 @@
       <c r="BH142" s="1">
         <v>1.8722483809999999E-2</v>
       </c>
+      <c r="BI142" s="1">
+        <v>28</v>
+      </c>
+      <c r="BJ142" s="1">
+        <v>-1.396565121E-3</v>
+      </c>
+      <c r="BK142" s="1">
+        <v>-5.534024502E-3</v>
+      </c>
     </row>
-    <row r="143" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>28.2</v>
       </c>
@@ -26599,8 +27886,17 @@
       <c r="BH143" s="1">
         <v>1.8903914420000001E-2</v>
       </c>
+      <c r="BI143" s="1">
+        <v>28.2</v>
+      </c>
+      <c r="BJ143" s="1">
+        <v>-2.4183417400000001E-3</v>
+      </c>
+      <c r="BK143" s="1">
+        <v>-5.0155442589999997E-3</v>
+      </c>
     </row>
-    <row r="144" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>28.4</v>
       </c>
@@ -26781,8 +28077,17 @@
       <c r="BH144" s="1">
         <v>1.979251261E-2</v>
       </c>
+      <c r="BI144" s="1">
+        <v>28.4</v>
+      </c>
+      <c r="BJ144" s="1">
+        <v>-1.790217651E-3</v>
+      </c>
+      <c r="BK144" s="1">
+        <v>-4.2160766129999997E-3</v>
+      </c>
     </row>
-    <row r="145" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>28.6</v>
       </c>
@@ -26963,8 +28268,17 @@
       <c r="BH145" s="1">
         <v>1.9710208310000001E-2</v>
       </c>
+      <c r="BI145" s="1">
+        <v>28.6</v>
+      </c>
+      <c r="BJ145" s="1">
+        <v>-7.0625789460000005E-4</v>
+      </c>
+      <c r="BK145" s="1">
+        <v>-3.7057505219999999E-3</v>
+      </c>
     </row>
-    <row r="146" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>28.8</v>
       </c>
@@ -27145,8 +28459,17 @@
       <c r="BH146" s="1">
         <v>1.9127461660000001E-2</v>
       </c>
+      <c r="BI146" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="BJ146" s="1">
+        <v>-2.3638517540000002E-3</v>
+      </c>
+      <c r="BK146" s="1">
+        <v>-3.6403648229999998E-3</v>
+      </c>
     </row>
-    <row r="147" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>29</v>
       </c>
@@ -27327,8 +28650,17 @@
       <c r="BH147" s="1">
         <v>1.8342378749999999E-2</v>
       </c>
+      <c r="BI147" s="1">
+        <v>29</v>
+      </c>
+      <c r="BJ147" s="1">
+        <v>-2.417498683E-3</v>
+      </c>
+      <c r="BK147" s="1">
+        <v>-3.872778089E-3</v>
+      </c>
     </row>
-    <row r="148" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>29.2</v>
       </c>
@@ -27509,8 +28841,17 @@
       <c r="BH148" s="1">
         <v>1.77233189E-2</v>
       </c>
+      <c r="BI148" s="1">
+        <v>29.2</v>
+      </c>
+      <c r="BJ148" s="1">
+        <v>-7.6846387609999999E-4</v>
+      </c>
+      <c r="BK148" s="1">
+        <v>-5.037725063E-3</v>
+      </c>
     </row>
-    <row r="149" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>29.4</v>
       </c>
@@ -27691,8 +29032,17 @@
       <c r="BH149" s="1">
         <v>1.8382959149999999E-2</v>
       </c>
+      <c r="BI149" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="BJ149" s="1">
+        <v>-7.0170387640000002E-4</v>
+      </c>
+      <c r="BK149" s="1">
+        <v>-5.0241821130000003E-3</v>
+      </c>
     </row>
-    <row r="150" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>29.6</v>
       </c>
@@ -27873,8 +29223,17 @@
       <c r="BH150" s="1">
         <v>1.7605717409999999E-2</v>
       </c>
+      <c r="BI150" s="1">
+        <v>29.6</v>
+      </c>
+      <c r="BJ150" s="1">
+        <v>-3.0016199370000001E-4</v>
+      </c>
+      <c r="BK150" s="1">
+        <v>-3.7245064790000001E-3</v>
+      </c>
     </row>
-    <row r="151" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>29.8</v>
       </c>
@@ -28055,8 +29414,17 @@
       <c r="BH151" s="1">
         <v>1.6285147619999999E-2</v>
       </c>
+      <c r="BI151" s="1">
+        <v>29.8</v>
+      </c>
+      <c r="BJ151" s="1">
+        <v>-3.01327975E-4</v>
+      </c>
+      <c r="BK151" s="1">
+        <v>-3.4406683519999999E-3</v>
+      </c>
     </row>
-    <row r="152" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>30</v>
       </c>
@@ -28237,8 +29605,17 @@
       <c r="BH152" s="1">
         <v>1.654553668E-2</v>
       </c>
+      <c r="BI152" s="1">
+        <v>30</v>
+      </c>
+      <c r="BJ152" s="1">
+        <v>-1.9946687259999999E-4</v>
+      </c>
+      <c r="BK152" s="1">
+        <v>-4.664399554E-3</v>
+      </c>
     </row>
-    <row r="153" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>30.2</v>
       </c>
@@ -28419,8 +29796,17 @@
       <c r="BH153" s="1">
         <v>1.570901534E-2</v>
       </c>
+      <c r="BI153" s="1">
+        <v>30.2</v>
+      </c>
+      <c r="BJ153" s="1">
+        <v>4.393898066E-4</v>
+      </c>
+      <c r="BK153" s="1">
+        <v>-3.9453043450000001E-3</v>
+      </c>
     </row>
-    <row r="154" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>30.4</v>
       </c>
@@ -28601,8 +29987,17 @@
       <c r="BH154" s="1">
         <v>1.540807284E-2</v>
       </c>
+      <c r="BI154" s="1">
+        <v>30.4</v>
+      </c>
+      <c r="BJ154" s="1">
+        <v>7.8290554670000002E-4</v>
+      </c>
+      <c r="BK154" s="1">
+        <v>-3.7155051349999999E-3</v>
+      </c>
     </row>
-    <row r="155" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>30.6</v>
       </c>
@@ -28783,8 +30178,17 @@
       <c r="BH155" s="1">
         <v>1.5538794430000001E-2</v>
       </c>
+      <c r="BI155" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="BJ155" s="1">
+        <v>-1.3569265399999999E-4</v>
+      </c>
+      <c r="BK155" s="1">
+        <v>-5.1205844970000003E-3</v>
+      </c>
     </row>
-    <row r="156" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>30.8</v>
       </c>
@@ -28965,8 +30369,17 @@
       <c r="BH156" s="1">
         <v>1.552651851E-2</v>
       </c>
+      <c r="BI156" s="1">
+        <v>30.8</v>
+      </c>
+      <c r="BJ156" s="1">
+        <v>-6.5186751530000003E-4</v>
+      </c>
+      <c r="BK156" s="1">
+        <v>-5.933140321E-3</v>
+      </c>
     </row>
-    <row r="157" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>31</v>
       </c>
@@ -29147,8 +30560,17 @@
       <c r="BH157" s="1">
         <v>1.4123916550000001E-2</v>
       </c>
+      <c r="BI157" s="1">
+        <v>31</v>
+      </c>
+      <c r="BJ157" s="1">
+        <v>3.4530629589999997E-5</v>
+      </c>
+      <c r="BK157" s="1">
+        <v>-5.1393751149999998E-3</v>
+      </c>
     </row>
-    <row r="158" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>31.2</v>
       </c>
@@ -29329,8 +30751,17 @@
       <c r="BH158" s="1">
         <v>1.3249953849999999E-2</v>
       </c>
+      <c r="BI158" s="1">
+        <v>31.2</v>
+      </c>
+      <c r="BJ158" s="1">
+        <v>-1.0521683509999999E-3</v>
+      </c>
+      <c r="BK158" s="1">
+        <v>-4.2659486660000003E-3</v>
+      </c>
     </row>
-    <row r="159" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>31.4</v>
       </c>
@@ -29511,8 +30942,17 @@
       <c r="BH159" s="1">
         <v>1.1322080809999999E-2</v>
       </c>
+      <c r="BI159" s="1">
+        <v>31.4</v>
+      </c>
+      <c r="BJ159" s="1">
+        <v>1.4227853840000001E-4</v>
+      </c>
+      <c r="BK159" s="1">
+        <v>-3.1762230659999999E-3</v>
+      </c>
     </row>
-    <row r="160" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>31.6</v>
       </c>
@@ -29693,8 +31133,17 @@
       <c r="BH160" s="1">
         <v>1.2217395900000001E-2</v>
       </c>
+      <c r="BI160" s="1">
+        <v>31.6</v>
+      </c>
+      <c r="BJ160" s="1">
+        <v>-1.4384726939999999E-3</v>
+      </c>
+      <c r="BK160" s="1">
+        <v>-3.617270237E-3</v>
+      </c>
     </row>
-    <row r="161" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>31.8</v>
       </c>
@@ -29875,8 +31324,17 @@
       <c r="BH161" s="1">
         <v>1.0848868540000001E-2</v>
       </c>
+      <c r="BI161" s="1">
+        <v>31.8</v>
+      </c>
+      <c r="BJ161" s="1">
+        <v>-4.1895539810000004E-3</v>
+      </c>
+      <c r="BK161" s="1">
+        <v>-2.9456112470000002E-3</v>
+      </c>
     </row>
-    <row r="162" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>32</v>
       </c>
@@ -30057,8 +31515,17 @@
       <c r="BH162" s="1">
         <v>1.0243264219999999E-2</v>
       </c>
+      <c r="BI162" s="1">
+        <v>32</v>
+      </c>
+      <c r="BJ162" s="1">
+        <v>-4.2411448759999996E-3</v>
+      </c>
+      <c r="BK162" s="1">
+        <v>-2.1640237079999999E-3</v>
+      </c>
     </row>
-    <row r="163" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>32.200000000000003</v>
       </c>
@@ -30239,8 +31706,17 @@
       <c r="BH163" s="1">
         <v>9.8206795610000005E-3</v>
       </c>
+      <c r="BI163" s="1">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="BJ163" s="1">
+        <v>-4.1404053160000003E-3</v>
+      </c>
+      <c r="BK163" s="1">
+        <v>-1.736577104E-3</v>
+      </c>
     </row>
-    <row r="164" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>32.4</v>
       </c>
@@ -30421,8 +31897,17 @@
       <c r="BH164" s="1">
         <v>1.203198292E-2</v>
       </c>
+      <c r="BI164" s="1">
+        <v>32.4</v>
+      </c>
+      <c r="BJ164" s="1">
+        <v>-2.6950233529999998E-3</v>
+      </c>
+      <c r="BK164" s="1">
+        <v>-2.1287935080000001E-3</v>
+      </c>
     </row>
-    <row r="165" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>32.6</v>
       </c>
@@ -30603,8 +32088,17 @@
       <c r="BH165" s="1">
         <v>1.200252418E-2</v>
       </c>
+      <c r="BI165" s="1">
+        <v>32.6</v>
+      </c>
+      <c r="BJ165" s="1">
+        <v>-5.5577842829999998E-3</v>
+      </c>
+      <c r="BK165" s="1">
+        <v>-7.2871779519999996E-4</v>
+      </c>
     </row>
-    <row r="166" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>32.799999999999997</v>
       </c>
@@ -30785,8 +32279,17 @@
       <c r="BH166" s="1">
         <v>1.1775642960000001E-2</v>
       </c>
+      <c r="BI166" s="1">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="BJ166" s="1">
+        <v>-4.6434120540000002E-3</v>
+      </c>
+      <c r="BK166" s="1">
+        <v>-6.8056676049999996E-4</v>
+      </c>
     </row>
-    <row r="167" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>33</v>
       </c>
@@ -30967,8 +32470,17 @@
       <c r="BH167" s="1">
         <v>1.134789852E-2</v>
       </c>
+      <c r="BI167" s="1">
+        <v>33</v>
+      </c>
+      <c r="BJ167" s="1">
+        <v>-5.1653206320000002E-3</v>
+      </c>
+      <c r="BK167" s="1">
+        <v>-4.8548533490000003E-5</v>
+      </c>
     </row>
-    <row r="168" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>33.200000000000003</v>
       </c>
@@ -31149,8 +32661,17 @@
       <c r="BH168" s="1">
         <v>9.7562066739999998E-3</v>
       </c>
+      <c r="BI168" s="1">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="BJ168" s="1">
+        <v>-4.6457960119999997E-3</v>
+      </c>
+      <c r="BK168" s="1">
+        <v>-1.641265381E-3</v>
+      </c>
     </row>
-    <row r="169" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>33.4</v>
       </c>
@@ -31331,8 +32852,17 @@
       <c r="BH169" s="1">
         <v>9.0142902709999997E-3</v>
       </c>
+      <c r="BI169" s="1">
+        <v>33.4</v>
+      </c>
+      <c r="BJ169" s="1">
+        <v>-3.3300968569999999E-3</v>
+      </c>
+      <c r="BK169" s="1">
+        <v>-1.5974498189999999E-3</v>
+      </c>
     </row>
-    <row r="170" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>33.6</v>
       </c>
@@ -31513,8 +33043,17 @@
       <c r="BH170" s="1">
         <v>8.2365909940000006E-3</v>
       </c>
+      <c r="BI170" s="1">
+        <v>33.6</v>
+      </c>
+      <c r="BJ170" s="1">
+        <v>-2.4112846520000001E-3</v>
+      </c>
+      <c r="BK170" s="1">
+        <v>-7.0012465190000001E-4</v>
+      </c>
     </row>
-    <row r="171" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>33.799999999999997</v>
       </c>
@@ -31695,8 +33234,17 @@
       <c r="BH171" s="1">
         <v>9.5767795780000008E-3</v>
       </c>
+      <c r="BI171" s="1">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="BJ171" s="1">
+        <v>8.9400069189999993E-5</v>
+      </c>
+      <c r="BK171" s="1">
+        <v>1.886776629E-4</v>
+      </c>
     </row>
-    <row r="172" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>34</v>
       </c>
@@ -31877,8 +33425,17 @@
       <c r="BH172" s="1">
         <v>1.023971106E-2</v>
       </c>
+      <c r="BI172" s="1">
+        <v>34</v>
+      </c>
+      <c r="BJ172" s="1">
+        <v>8.9265498430000001E-4</v>
+      </c>
+      <c r="BK172" s="1">
+        <v>-1.013617176E-3</v>
+      </c>
     </row>
-    <row r="173" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>34.200000000000003</v>
       </c>
@@ -32059,8 +33616,17 @@
       <c r="BH173" s="1">
         <v>1.2587776259999999E-2</v>
       </c>
+      <c r="BI173" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="BJ173" s="1">
+        <v>2.139742218E-3</v>
+      </c>
+      <c r="BK173" s="1">
+        <v>-8.0250302810000001E-5</v>
+      </c>
     </row>
-    <row r="174" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>34.4</v>
       </c>
@@ -32241,8 +33807,17 @@
       <c r="BH174" s="1">
         <v>1.339167961E-2</v>
       </c>
+      <c r="BI174" s="1">
+        <v>34.4</v>
+      </c>
+      <c r="BJ174" s="1">
+        <v>2.3206355969999999E-3</v>
+      </c>
+      <c r="BK174" s="1">
+        <v>-4.0300370850000002E-4</v>
+      </c>
     </row>
-    <row r="175" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>34.6</v>
       </c>
@@ -32423,8 +33998,17 @@
       <c r="BH175" s="1">
         <v>1.511683011E-2</v>
       </c>
+      <c r="BI175" s="1">
+        <v>34.6</v>
+      </c>
+      <c r="BJ175" s="1">
+        <v>1.462614123E-3</v>
+      </c>
+      <c r="BK175" s="1">
+        <v>-5.6955150999999998E-4</v>
+      </c>
     </row>
-    <row r="176" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>34.799999999999997</v>
       </c>
@@ -32605,8 +34189,17 @@
       <c r="BH176" s="1">
         <v>1.59579779E-2</v>
       </c>
+      <c r="BI176" s="1">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="BJ176" s="1">
+        <v>6.6618320610000001E-4</v>
+      </c>
+      <c r="BK176" s="1">
+        <v>-3.4849262930000002E-4</v>
+      </c>
     </row>
-    <row r="177" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>35</v>
       </c>
@@ -32787,8 +34380,17 @@
       <c r="BH177" s="1">
         <v>1.560288606E-2</v>
       </c>
+      <c r="BI177" s="1">
+        <v>35</v>
+      </c>
+      <c r="BJ177" s="1">
+        <v>-1.4488935030000001E-3</v>
+      </c>
+      <c r="BK177" s="1">
+        <v>-2.0386113579999999E-3</v>
+      </c>
     </row>
-    <row r="178" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>35.200000000000003</v>
       </c>
@@ -32969,8 +34571,17 @@
       <c r="BH178" s="1">
         <v>1.5700084E-2</v>
       </c>
+      <c r="BI178" s="1">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="BJ178" s="1">
+        <v>-7.0994319710000005E-4</v>
+      </c>
+      <c r="BK178" s="1">
+        <v>-2.8259713130000001E-3</v>
+      </c>
     </row>
-    <row r="179" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>35.4</v>
       </c>
@@ -33151,8 +34762,17 @@
       <c r="BH179" s="1">
         <v>1.452066739E-2</v>
       </c>
+      <c r="BI179" s="1">
+        <v>35.4</v>
+      </c>
+      <c r="BJ179" s="1">
+        <v>-9.9353178379999992E-4</v>
+      </c>
+      <c r="BK179" s="1">
+        <v>-2.4955791469999998E-3</v>
+      </c>
     </row>
-    <row r="180" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>35.6</v>
       </c>
@@ -33333,8 +34953,17 @@
       <c r="BH180" s="1">
         <v>1.355737246E-2</v>
       </c>
+      <c r="BI180" s="1">
+        <v>35.6</v>
+      </c>
+      <c r="BJ180" s="1">
+        <v>-3.0842152390000001E-4</v>
+      </c>
+      <c r="BK180" s="1">
+        <v>-2.4435409650000002E-3</v>
+      </c>
     </row>
-    <row r="181" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>35.799999999999997</v>
       </c>
@@ -33515,8 +35144,17 @@
       <c r="BH181" s="1">
         <v>1.2587199069999999E-2</v>
       </c>
+      <c r="BI181" s="1">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="BJ181" s="1">
+        <v>6.6489585690000005E-4</v>
+      </c>
+      <c r="BK181" s="1">
+        <v>-3.4250919759999999E-3</v>
+      </c>
     </row>
-    <row r="182" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>36</v>
       </c>
@@ -33697,8 +35335,17 @@
       <c r="BH182" s="1">
         <v>1.203222786E-2</v>
       </c>
+      <c r="BI182" s="1">
+        <v>36</v>
+      </c>
+      <c r="BJ182" s="1">
+        <v>1.1199644640000001E-3</v>
+      </c>
+      <c r="BK182" s="1">
+        <v>-4.2631169900000003E-3</v>
+      </c>
     </row>
-    <row r="183" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>36.200000000000003</v>
       </c>
@@ -33879,8 +35526,17 @@
       <c r="BH183" s="1">
         <v>1.323510522E-2</v>
       </c>
+      <c r="BI183" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="BJ183" s="1">
+        <v>9.5992694009999993E-5</v>
+      </c>
+      <c r="BK183" s="1">
+        <v>-4.4533551989999996E-3</v>
+      </c>
     </row>
-    <row r="184" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>36.4</v>
       </c>
@@ -34061,8 +35717,17 @@
       <c r="BH184" s="1">
         <v>1.164454541E-2</v>
       </c>
+      <c r="BI184" s="1">
+        <v>36.4</v>
+      </c>
+      <c r="BJ184" s="1">
+        <v>-1.854702959E-5</v>
+      </c>
+      <c r="BK184" s="1">
+        <v>-5.2039832769999999E-3</v>
+      </c>
     </row>
-    <row r="185" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>36.6</v>
       </c>
@@ -34243,8 +35908,17 @@
       <c r="BH185" s="1">
         <v>1.1386963119999999E-2</v>
       </c>
+      <c r="BI185" s="1">
+        <v>36.6</v>
+      </c>
+      <c r="BJ185" s="1">
+        <v>-3.0281731730000001E-4</v>
+      </c>
+      <c r="BK185" s="1">
+        <v>-4.8633444140000004E-3</v>
+      </c>
     </row>
-    <row r="186" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>36.799999999999997</v>
       </c>
@@ -34425,8 +36099,17 @@
       <c r="BH186" s="1">
         <v>1.1804799100000001E-2</v>
       </c>
+      <c r="BI186" s="1">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="BJ186" s="1">
+        <v>-1.3358366770000001E-3</v>
+      </c>
+      <c r="BK186" s="1">
+        <v>-4.0444395519999999E-3</v>
+      </c>
     </row>
-    <row r="187" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>37</v>
       </c>
@@ -34607,8 +36290,17 @@
       <c r="BH187" s="1">
         <v>1.1505479399999999E-2</v>
       </c>
+      <c r="BI187" s="1">
+        <v>37</v>
+      </c>
+      <c r="BJ187" s="1">
+        <v>-1.3497534430000001E-4</v>
+      </c>
+      <c r="BK187" s="1">
+        <v>-5.1863825849999996E-3</v>
+      </c>
     </row>
-    <row r="188" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>37.200000000000003</v>
       </c>
@@ -34789,8 +36481,17 @@
       <c r="BH188" s="1">
         <v>9.7922065409999995E-3</v>
       </c>
+      <c r="BI188" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="BJ188" s="1">
+        <v>5.4595804330000001E-4</v>
+      </c>
+      <c r="BK188" s="1">
+        <v>-4.5685574599999999E-3</v>
+      </c>
     </row>
-    <row r="189" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>37.4</v>
       </c>
@@ -34971,8 +36672,17 @@
       <c r="BH189" s="1">
         <v>1.0752525670000001E-2</v>
       </c>
+      <c r="BI189" s="1">
+        <v>37.4</v>
+      </c>
+      <c r="BJ189" s="1">
+        <v>1.3584686239999999E-3</v>
+      </c>
+      <c r="BK189" s="1">
+        <v>-4.8358703580000002E-3</v>
+      </c>
     </row>
-    <row r="190" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>37.6</v>
       </c>
@@ -35153,8 +36863,17 @@
       <c r="BH190" s="1">
         <v>1.022888341E-2</v>
       </c>
+      <c r="BI190" s="1">
+        <v>37.6</v>
+      </c>
+      <c r="BJ190" s="1">
+        <v>9.5198085490000002E-4</v>
+      </c>
+      <c r="BK190" s="1">
+        <v>-5.0832910510000004E-3</v>
+      </c>
     </row>
-    <row r="191" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>37.799999999999997</v>
       </c>
@@ -35335,8 +37054,17 @@
       <c r="BH191" s="1">
         <v>8.8115616479999999E-3</v>
       </c>
+      <c r="BI191" s="1">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="BJ191" s="1">
+        <v>5.9551974150000005E-4</v>
+      </c>
+      <c r="BK191" s="1">
+        <v>-5.0810636589999998E-3</v>
+      </c>
     </row>
-    <row r="192" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>38</v>
       </c>
@@ -35517,8 +37245,17 @@
       <c r="BH192" s="1">
         <v>8.6228842549999993E-3</v>
       </c>
+      <c r="BI192" s="1">
+        <v>38</v>
+      </c>
+      <c r="BJ192" s="1">
+        <v>2.7174063419999999E-4</v>
+      </c>
+      <c r="BK192" s="1">
+        <v>-3.4833815459999998E-3</v>
+      </c>
     </row>
-    <row r="193" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>38.200000000000003</v>
       </c>
@@ -35699,8 +37436,17 @@
       <c r="BH193" s="1">
         <v>6.9146011459999997E-3</v>
       </c>
+      <c r="BI193" s="1">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="BJ193" s="1">
+        <v>-7.6152194700000004E-4</v>
+      </c>
+      <c r="BK193" s="1">
+        <v>-2.6346691709999998E-3</v>
+      </c>
     </row>
-    <row r="194" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>38.4</v>
       </c>
@@ -35881,8 +37627,17 @@
       <c r="BH194" s="1">
         <v>8.7662234229999997E-3</v>
       </c>
+      <c r="BI194" s="1">
+        <v>38.4</v>
+      </c>
+      <c r="BJ194" s="1">
+        <v>-7.6091784810000001E-4</v>
+      </c>
+      <c r="BK194" s="1">
+        <v>-6.3591329899999999E-4</v>
+      </c>
     </row>
-    <row r="195" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>38.6</v>
       </c>
@@ -36063,8 +37818,17 @@
       <c r="BH195" s="1">
         <v>9.3799331590000007E-3</v>
       </c>
+      <c r="BI195" s="1">
+        <v>38.6</v>
+      </c>
+      <c r="BJ195" s="1">
+        <v>-2.4922228069999999E-5</v>
+      </c>
+      <c r="BK195" s="1">
+        <v>-9.60610021E-4</v>
+      </c>
     </row>
-    <row r="196" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>38.799999999999997</v>
       </c>
@@ -36245,8 +38009,17 @@
       <c r="BH196" s="1">
         <v>7.6810472479999998E-3</v>
       </c>
+      <c r="BI196" s="1">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="BJ196" s="1">
+        <v>-3.0242407670000001E-4</v>
+      </c>
+      <c r="BK196" s="1">
+        <v>-1.8320082859999999E-3</v>
+      </c>
     </row>
-    <row r="197" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>39</v>
       </c>
@@ -36427,8 +38200,17 @@
       <c r="BH197" s="1">
         <v>6.5615024620000002E-3</v>
       </c>
+      <c r="BI197" s="1">
+        <v>39</v>
+      </c>
+      <c r="BJ197" s="1">
+        <v>8.6517948510000006E-5</v>
+      </c>
+      <c r="BK197" s="1">
+        <v>-1.1644331989999999E-3</v>
+      </c>
     </row>
-    <row r="198" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>39.200000000000003</v>
       </c>
@@ -36609,8 +38391,17 @@
       <c r="BH198" s="1">
         <v>7.507755774E-3</v>
       </c>
+      <c r="BI198" s="1">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="BJ198" s="1">
+        <v>6.6794492399999995E-4</v>
+      </c>
+      <c r="BK198" s="1">
+        <v>-2.5733051729999999E-3</v>
+      </c>
     </row>
-    <row r="199" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>39.4</v>
       </c>
@@ -36791,8 +38582,17 @@
       <c r="BH199" s="1">
         <v>8.0796557949999997E-3</v>
       </c>
+      <c r="BI199" s="1">
+        <v>39.4</v>
+      </c>
+      <c r="BJ199" s="1">
+        <v>8.9857167750000003E-4</v>
+      </c>
+      <c r="BK199" s="1">
+        <v>-2.4081191310000001E-3</v>
+      </c>
     </row>
-    <row r="200" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>39.6</v>
       </c>
@@ -36973,8 +38773,17 @@
       <c r="BH200" s="1">
         <v>8.1245539329999998E-3</v>
       </c>
+      <c r="BI200" s="1">
+        <v>39.6</v>
+      </c>
+      <c r="BJ200" s="1">
+        <v>1.5170457959999999E-3</v>
+      </c>
+      <c r="BK200" s="1">
+        <v>-3.0788204660000002E-3</v>
+      </c>
     </row>
-    <row r="201" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>39.799999999999997</v>
       </c>
@@ -37130,6 +38939,15 @@
       </c>
       <c r="BH201" s="1">
         <v>9.075527311E-3</v>
+      </c>
+      <c r="BI201" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="BJ201" s="1">
+        <v>1.2326918749999999E-3</v>
+      </c>
+      <c r="BK201" s="1">
+        <v>-2.3681537110000002E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>